<commit_message>
Completed babble version of FST
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heard\Documents\GitHub\FST_PsychoPy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjh200002\Documents\GitHub\FST_PsychoPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893C17AC-1778-4530-834E-8FF1C6DC95BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE621873-C033-4B68-8BB9-10B62F02A8C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{FF7DADCE-7059-7745-AFCE-6BD90386092C}"/>
+    <workbookView xWindow="2700" yWindow="-105" windowWidth="22305" windowHeight="13170" xr2:uid="{FF7DADCE-7059-7745-AFCE-6BD90386092C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,42 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>sent_stim/094_SM.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/141_SM.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/141_SF.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/104_OF.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/104_OM.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/053_OF.wav</t>
-  </si>
-  <si>
-    <t>sent_stim/053_SF.wav</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>inst3</t>
   </si>
@@ -75,69 +45,99 @@
     <t>inst1</t>
   </si>
   <si>
-    <t>"Nephews that embrace nieces are suave"</t>
-  </si>
-  <si>
     <t>sent_stim</t>
   </si>
   <si>
-    <t>"Women that protect men are awesome."
-Who are performing the action?</t>
-  </si>
-  <si>
-    <t>"Men that protect women are awesome."
-Who are performing the action?</t>
-  </si>
-  <si>
-    <t>Since the MEN are doing the protecting, the answer is MEN.</t>
-  </si>
-  <si>
-    <t>Since the WOMEN are doing the protecting, the answer is WOMEN.</t>
-  </si>
-  <si>
     <t>Listen carefully to each sentence and pay attention to *who* is performing the action.</t>
   </si>
   <si>
-    <t>Since QUEENS are doing the assisting, the answer is FEMALE.</t>
-  </si>
-  <si>
     <t>In this test, you need to identify the *GENDER* of the people performing the action.</t>
   </si>
   <si>
     <t>Let's listen to another example! Pay attention to which *GENDER* is performing the action.</t>
-  </si>
-  <si>
-    <t>Since KINGS are doing the assisting, the answer is MALE.</t>
-  </si>
-  <si>
-    <t>Since LADIES are doing the shielding, the answer is FEMALE.</t>
-  </si>
-  <si>
-    <t>Likewise, since LADIES are doing the shielding, the answer is also FEMALE.</t>
-  </si>
-  <si>
-    <t>If the gender of the people performing the action is MALE, press the LEFT ARROW key.
-If the gender of the people performing the action is FEMALE, press the RIGHT ARROW key.</t>
   </si>
   <si>
     <t>You will listen to sentences like this one. 
 If you need to adjust the volume to make the sound louder, please do so.</t>
   </si>
   <si>
-    <t>"Kings that queens assist are helpful."
+    <t>Sometimes it will sound like the sentence is spoken in an even noisier room, like this:</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\102_SM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\104_OF_SNR-2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\102_SM_SNR-2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\103_SM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\103_SF_SNR-2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\104_OM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\105_OF_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_121720\105_SF_SNR-2.wav</t>
+  </si>
+  <si>
+    <t>It may be difficult to understand what is being said, but please do your best.</t>
+  </si>
+  <si>
+    <t>If the gender of the people performing the action is MALE, press the RIGHT ARROW key.
+If the gender of the people performing the action is FEMALE, press the LEFT ARROW key.</t>
+  </si>
+  <si>
+    <t>"Brothers that defend sisters are brave."</t>
+  </si>
+  <si>
+    <t>"Fathers that update mothers are useful."
+Who are performing the action?</t>
+  </si>
+  <si>
+    <t>"Mothers that update fathers are useful."
+Who are performing the action?</t>
+  </si>
+  <si>
+    <t>"Gentlemen that ladies befriend are cheerful."
 What is the gender of the people performing the action?</t>
   </si>
   <si>
-    <t>"Queens that kings assist are helpful."
+    <t>"Ladies that gentlemen befriend are cheerful."
 What is the gender of the people performing the action?</t>
   </si>
   <si>
-    <t>"Gentlemen that ladies shield are mighty."
+    <t>Since LADIES are doing the befriending, the answer is FEMALE.</t>
+  </si>
+  <si>
+    <t>Since GENTLEMEN are doing the befriending, the answer is MALE.</t>
+  </si>
+  <si>
+    <t>"Husbands that wives bolster are favorable."
 What is the gender of the people performing the action?</t>
   </si>
   <si>
-    <t>"Ladies that shield gentlemen are mighty."
+    <t>"Wives that bolster husbands are favorable."
 What is the gender of the people performing the action?</t>
+  </si>
+  <si>
+    <t>Since WIVES are doing the bolstering, the answer is FEMALE.</t>
+  </si>
+  <si>
+    <t>Likewise, since WIVES are doing the bolstering, the answer is also FEMALE.</t>
+  </si>
+  <si>
+    <t>Since the FATHERS are doing the updating, the answer is FATHERS.</t>
+  </si>
+  <si>
+    <t>Since the MOTHERS are doing the updating, the answer is MOTHERS.</t>
   </si>
 </sst>
 </file>
@@ -173,11 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -498,131 +497,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F17E23C-A6F2-D84B-8983-0038B6CD49B1}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="139.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New stimuli, adjusting instructions
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjh200002\Documents\GitHub\FST_PsychoPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE621873-C033-4B68-8BB9-10B62F02A8C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47621530-5FFA-41A2-9124-421842933FA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="-105" windowWidth="22305" windowHeight="13170" xr2:uid="{FF7DADCE-7059-7745-AFCE-6BD90386092C}"/>
+    <workbookView xWindow="4560" yWindow="-105" windowWidth="22305" windowHeight="13170" xr2:uid="{FF7DADCE-7059-7745-AFCE-6BD90386092C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,47 +48,10 @@
     <t>sent_stim</t>
   </si>
   <si>
-    <t>Listen carefully to each sentence and pay attention to *who* is performing the action.</t>
-  </si>
-  <si>
     <t>In this test, you need to identify the *GENDER* of the people performing the action.</t>
   </si>
   <si>
     <t>Let's listen to another example! Pay attention to which *GENDER* is performing the action.</t>
-  </si>
-  <si>
-    <t>You will listen to sentences like this one. 
-If you need to adjust the volume to make the sound louder, please do so.</t>
-  </si>
-  <si>
-    <t>Sometimes it will sound like the sentence is spoken in an even noisier room, like this:</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\102_SM_SNR2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\104_OF_SNR-2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\102_SM_SNR-2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\103_SM_SNR2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\103_SF_SNR-2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\104_OM_SNR2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\105_OF_SNR2.wav</t>
-  </si>
-  <si>
-    <t>sent_stim_121720\105_SF_SNR-2.wav</t>
-  </si>
-  <si>
-    <t>It may be difficult to understand what is being said, but please do your best.</t>
   </si>
   <si>
     <t>If the gender of the people performing the action is MALE, press the RIGHT ARROW key.
@@ -138,6 +101,45 @@
   </si>
   <si>
     <t>Since the MOTHERS are doing the updating, the answer is MOTHERS.</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\102_SM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\103_SM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\104_OM_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\105_OF_SNR2.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\102_SM_SNR2_0.5.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\103_SF_SNR2_0.5.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\104_OF_SNR2_0.5.wav</t>
+  </si>
+  <si>
+    <t>sent_stim_122220\105_SF_SNR2_0.5.wav</t>
+  </si>
+  <si>
+    <t>Sometimes the sentences will be louder, like this:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will listen to sentences like this one. 
+</t>
+  </si>
+  <si>
+    <t>It may be difficult to understand what is being said, but please do your best.
+'Listen carefully to each sentence and pay attention to *who* is performing the action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you need to adjust the volume to make the sound louder, please do so now.
+After you have found a comfortable volume level, stop adjusting the volume. </t>
   </si>
 </sst>
 </file>
@@ -499,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F17E23C-A6F2-D84B-8983-0038B6CD49B1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -528,114 +530,114 @@
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>